<commit_message>
add external workbook resolution in formula
</commit_message>
<xml_diff>
--- a/t/regression/xlsx_files/formulashared.xlsx
+++ b/t/regression/xlsx_files/formulashared.xlsx
@@ -11,6 +11,10 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
@@ -62,8 +66,54 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="Sheet4"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1">
+        <row r="3">
+          <cell r="C3">
+            <v>5</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1">
+            <v>1234</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -349,13 +399,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
@@ -430,7 +480,7 @@
       </c>
       <c r="D4">
         <f t="shared" si="2"/>
-        <v>81</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -550,6 +600,16 @@
       <c r="D11">
         <f t="shared" si="2"/>
         <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>A1+42+[1]Sheet1!$C$3</f>
+        <v>57</v>
+      </c>
+      <c r="B13">
+        <f>B1+42+[2]Sheet1!$A$1</f>
+        <v>1277</v>
       </c>
     </row>
   </sheetData>
@@ -563,7 +623,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -575,7 +635,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>